<commit_message>
json data sanitized and exported to excel
</commit_message>
<xml_diff>
--- a/data_files/city_data/Espoo.xlsx
+++ b/data_files/city_data/Espoo.xlsx
@@ -468,17 +468,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Meal, Inexpensive Restaurant</t>
+          <t>Meal Inexpensive Restaurant</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>16</v>
+        <v>1600</v>
       </c>
       <c r="D2" t="n">
-        <v>11</v>
+        <v>1100</v>
       </c>
       <c r="E2" t="n">
-        <v>20</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="3">
@@ -489,17 +489,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Meal for 2 People, Mid-range Restaurant, Three-course</t>
+          <t>Meal for 2 People Midrange Restaurant Threecourse</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>105</v>
+        <v>10500</v>
       </c>
       <c r="D3" t="n">
-        <v>70</v>
+        <v>7000</v>
       </c>
       <c r="E3" t="n">
-        <v>120</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="4">
@@ -510,17 +510,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>McMeal at McDonalds (or Equivalent Combo Meal)</t>
+          <t>McMeal at McDonalds or Equivalent Combo Meal</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="D4" t="n">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="E4" t="n">
-        <v>11</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="5">
@@ -531,17 +531,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Domestic Beer (0.5 liter draught)</t>
+          <t>Domestic Beer 05 liter draught</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>9</v>
+        <v>900</v>
       </c>
       <c r="D5" t="n">
-        <v>6</v>
+        <v>600</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="6">
@@ -552,17 +552,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Imported Beer (0.33 liter bottle)</t>
+          <t>Imported Beer 033 liter bottle</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>9</v>
+        <v>900</v>
       </c>
       <c r="D6" t="n">
-        <v>6</v>
+        <v>600</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="7">
@@ -573,17 +573,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Cappuccino (regular)</t>
+          <t>Cappuccino regular</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>4.79</v>
+        <v>479</v>
       </c>
       <c r="D7" t="n">
-        <v>3.5</v>
+        <v>350</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>600</v>
       </c>
     </row>
     <row r="8">
@@ -594,17 +594,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Coke/Pepsi (0.33 liter bottle)</t>
+          <t>CokePepsi 033 liter bottle</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>2.95</v>
+        <v>295</v>
       </c>
       <c r="D8" t="n">
-        <v>2.05</v>
+        <v>205</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>400</v>
       </c>
     </row>
     <row r="9">
@@ -615,17 +615,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Water (0.33 liter bottle)</t>
+          <t>Water 033 liter bottle</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2.43</v>
+        <v>243</v>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10">
@@ -636,17 +636,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Milk (regular), (1 liter)</t>
+          <t>Milk regular 1 liter</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1.15</v>
+        <v>115</v>
       </c>
       <c r="D10" t="n">
-        <v>0.83</v>
+        <v>83</v>
       </c>
       <c r="E10" t="n">
-        <v>1.5</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11">
@@ -657,17 +657,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Loaf of Fresh White Bread (500g)</t>
+          <t>Loaf of Fresh White Bread 500g</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>3.5</v>
+        <v>350</v>
       </c>
       <c r="D11" t="n">
-        <v>1.39</v>
+        <v>139</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>500</v>
       </c>
     </row>
     <row r="12">
@@ -678,17 +678,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Rice (white), (1kg)</t>
+          <t>Rice white 1kg</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>2.86</v>
+        <v>286</v>
       </c>
       <c r="D12" t="n">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="E12" t="n">
-        <v>4.35</v>
+        <v>435</v>
       </c>
     </row>
     <row r="13">
@@ -699,17 +699,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Eggs (regular) (12)</t>
+          <t>Eggs regular 12</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>3.53</v>
+        <v>353</v>
       </c>
       <c r="D13" t="n">
-        <v>2.03</v>
+        <v>203</v>
       </c>
       <c r="E13" t="n">
-        <v>4.8</v>
+        <v>480</v>
       </c>
     </row>
     <row r="14">
@@ -720,17 +720,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Local Cheese (1kg)</t>
+          <t>Local Cheese 1kg</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>8.75</v>
+        <v>875</v>
       </c>
       <c r="D14" t="n">
-        <v>5.95</v>
+        <v>595</v>
       </c>
       <c r="E14" t="n">
-        <v>14</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="15">
@@ -741,17 +741,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Chicken Fillets (1kg)</t>
+          <t>Chicken Fillets 1kg</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>12.18</v>
+        <v>1218</v>
       </c>
       <c r="D15" t="n">
-        <v>7.99</v>
+        <v>799</v>
       </c>
       <c r="E15" t="n">
-        <v>14</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="16">
@@ -762,17 +762,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Beef Round (1kg) (or Equivalent Back Leg Red Meat)</t>
+          <t>Beef Round 1kg or Equivalent Back Leg Red Meat</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>20.05</v>
+        <v>2005</v>
       </c>
       <c r="D16" t="n">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="E16" t="n">
-        <v>25</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="17">
@@ -783,17 +783,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Apples (1kg)</t>
+          <t>Apples 1kg</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>2.92</v>
+        <v>292</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>400</v>
       </c>
     </row>
     <row r="18">
@@ -804,17 +804,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Banana (1kg)</t>
+          <t>Banana 1kg</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1.85</v>
+        <v>185</v>
       </c>
       <c r="D18" t="n">
-        <v>1.25</v>
+        <v>125</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>500</v>
       </c>
     </row>
     <row r="19">
@@ -825,17 +825,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Oranges (1kg)</t>
+          <t>Oranges 1kg</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2.97</v>
+        <v>297</v>
       </c>
       <c r="D19" t="n">
-        <v>1.2</v>
+        <v>120</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>400</v>
       </c>
     </row>
     <row r="20">
@@ -846,17 +846,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Tomato (1kg)</t>
+          <t>Tomato 1kg</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>4.57</v>
+        <v>457</v>
       </c>
       <c r="D20" t="n">
-        <v>2.2</v>
+        <v>220</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>600</v>
       </c>
     </row>
     <row r="21">
@@ -867,17 +867,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Potato (1kg)</t>
+          <t>Potato 1kg</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1.29</v>
+        <v>129</v>
       </c>
       <c r="D21" t="n">
-        <v>0.75</v>
+        <v>75</v>
       </c>
       <c r="E21" t="n">
-        <v>2.4</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22">
@@ -888,17 +888,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Onion (1kg)</t>
+          <t>Onion 1kg</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1.72</v>
+        <v>172</v>
       </c>
       <c r="D22" t="n">
-        <v>1.3</v>
+        <v>130</v>
       </c>
       <c r="E22" t="n">
-        <v>2.71</v>
+        <v>271</v>
       </c>
     </row>
     <row r="23">
@@ -909,17 +909,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Lettuce (1 head)</t>
+          <t>Lettuce 1 head</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1.88</v>
+        <v>188</v>
       </c>
       <c r="D23" t="n">
-        <v>1.39</v>
+        <v>139</v>
       </c>
       <c r="E23" t="n">
-        <v>2.2</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24">
@@ -930,17 +930,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Water (1.5 liter bottle)</t>
+          <t>Water 15 liter bottle</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2.08</v>
+        <v>208</v>
       </c>
       <c r="D24" t="n">
-        <v>1.17</v>
+        <v>117</v>
       </c>
       <c r="E24" t="n">
-        <v>2.5</v>
+        <v>250</v>
       </c>
     </row>
     <row r="25">
@@ -951,17 +951,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Bottle of Wine (Mid-Range)</t>
+          <t>Bottle of Wine MidRange</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>15</v>
+        <v>1500</v>
       </c>
       <c r="D25" t="n">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="E25" t="n">
-        <v>18</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="26">
@@ -972,17 +972,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Domestic Beer (0.5 liter bottle)</t>
+          <t>Domestic Beer 05 liter bottle</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>3.51</v>
+        <v>351</v>
       </c>
       <c r="D26" t="n">
-        <v>2.5</v>
+        <v>250</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>400</v>
       </c>
     </row>
     <row r="27">
@@ -993,17 +993,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Imported Beer (0.33 liter bottle)</t>
+          <t>Imported Beer 033 liter bottle</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>4.14</v>
+        <v>414</v>
       </c>
       <c r="D27" t="n">
-        <v>3</v>
+        <v>300</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>500</v>
       </c>
     </row>
     <row r="28">
@@ -1014,17 +1014,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Cigarettes 20 Pack (Marlboro)</t>
+          <t>Cigarettes 20 Pack Marlboro</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>11</v>
+        <v>1100</v>
       </c>
       <c r="D28" t="n">
-        <v>9.949999999999999</v>
+        <v>995</v>
       </c>
       <c r="E28" t="n">
-        <v>11</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="29">
@@ -1035,17 +1035,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>One-way Ticket (Local Transport)</t>
+          <t>Oneway Ticket Local Transport</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3</v>
+        <v>300</v>
       </c>
       <c r="D29" t="n">
-        <v>2.8</v>
+        <v>280</v>
       </c>
       <c r="E29" t="n">
-        <v>3.1</v>
+        <v>310</v>
       </c>
     </row>
     <row r="30">
@@ -1056,17 +1056,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Monthly Pass (Regular Price)</t>
+          <t>Monthly Pass Regular Price</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>70</v>
+        <v>7000</v>
       </c>
       <c r="D30" t="n">
-        <v>60</v>
+        <v>6000</v>
       </c>
       <c r="E30" t="n">
-        <v>99</v>
+        <v>9900</v>
       </c>
     </row>
     <row r="31">
@@ -1077,17 +1077,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Taxi Start (Normal Tariff)</t>
+          <t>Taxi Start Normal Tariff</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>8</v>
+        <v>800</v>
       </c>
       <c r="D31" t="n">
-        <v>6.5</v>
+        <v>650</v>
       </c>
       <c r="E31" t="n">
-        <v>10</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="32">
@@ -1098,17 +1098,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Taxi 1km (Normal Tariff)</t>
+          <t>Taxi 1km Normal Tariff</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1.5</v>
+        <v>150</v>
       </c>
       <c r="D32" t="n">
-        <v>1.2</v>
+        <v>120</v>
       </c>
       <c r="E32" t="n">
-        <v>1.99</v>
+        <v>199</v>
       </c>
     </row>
     <row r="33">
@@ -1119,17 +1119,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Taxi 1hour Waiting (Normal Tariff)</t>
+          <t>Taxi 1hour Waiting Normal Tariff</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>46</v>
+        <v>4600</v>
       </c>
       <c r="D33" t="n">
-        <v>44.4</v>
+        <v>4440</v>
       </c>
       <c r="E33" t="n">
-        <v>55</v>
+        <v>5500</v>
       </c>
     </row>
     <row r="34">
@@ -1140,17 +1140,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Gasoline (1 liter)</t>
+          <t>Gasoline 1 liter</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1.94</v>
+        <v>194</v>
       </c>
       <c r="D34" t="n">
-        <v>1.81</v>
+        <v>181</v>
       </c>
       <c r="E34" t="n">
-        <v>2.2</v>
+        <v>220</v>
       </c>
     </row>
     <row r="35">
@@ -1161,17 +1161,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Volkswagen Golf 1.4 90 KW Trendline (Or Equivalent New Car)</t>
+          <t>Volkswagen Golf 14 90 KW Trendline Or Equivalent New Car</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>28500</v>
+        <v>2850000</v>
       </c>
       <c r="D35" t="n">
-        <v>28000</v>
+        <v>2800000</v>
       </c>
       <c r="E35" t="n">
-        <v>28550</v>
+        <v>2855000</v>
       </c>
     </row>
     <row r="36">
@@ -1182,80 +1182,80 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Toyota Corolla Sedan 1.6l 97kW Comfort (Or Equivalent New Car)</t>
+          <t>Toyota Corolla Sedan 16l 97kW Comfort Or Equivalent New Car</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>30214.14</v>
+        <v>3021414</v>
       </c>
       <c r="D36" t="n">
-        <v>30000</v>
+        <v>3000000</v>
       </c>
       <c r="E36" t="n">
-        <v>30000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Utilities (Monthly)</t>
+          <t>Utilities Monthly</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Basic (Electricity, Heating, Cooling, Water, Garbage) for 85m2 Apartment</t>
+          <t>Basic Electricity Heating Cooling Water Garbage for 85m2 Apartment</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>106.01</v>
+        <v>10601</v>
       </c>
       <c r="D37" t="n">
-        <v>76</v>
+        <v>7600</v>
       </c>
       <c r="E37" t="n">
-        <v>200</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Utilities (Monthly)</t>
+          <t>Utilities Monthly</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Mobile Phone Monthly Plan with Calls and 10GB+ Data</t>
+          <t>Mobile Phone Monthly Plan with Calls and 10GB Data</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>26.85</v>
+        <v>2685</v>
       </c>
       <c r="D38" t="n">
-        <v>20</v>
+        <v>2000</v>
       </c>
       <c r="E38" t="n">
-        <v>26.99</v>
+        <v>2699</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Utilities (Monthly)</t>
+          <t>Utilities Monthly</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Internet (60 Mbps or More, Unlimited Data, Cable/ADSL)</t>
+          <t>Internet 60 Mbps or More Unlimited Data CableADSL</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>18.13</v>
+        <v>1813</v>
       </c>
       <c r="D39" t="n">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="E39" t="n">
-        <v>25</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="40">
@@ -1266,17 +1266,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Fitness Club, Monthly Fee for 1 Adult</t>
+          <t>Fitness Club Monthly Fee for 1 Adult</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>53.41</v>
+        <v>5341</v>
       </c>
       <c r="D40" t="n">
-        <v>29</v>
+        <v>2900</v>
       </c>
       <c r="E40" t="n">
-        <v>65</v>
+        <v>6500</v>
       </c>
     </row>
     <row r="41">
@@ -1287,17 +1287,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Tennis Court Rent (1 Hour on Weekend)</t>
+          <t>Tennis Court Rent 1 Hour on Weekend</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>32.44</v>
+        <v>3244</v>
       </c>
       <c r="D41" t="n">
-        <v>25</v>
+        <v>2500</v>
       </c>
       <c r="E41" t="n">
-        <v>35</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="42">
@@ -1308,17 +1308,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Cinema, International Release, 1 Seat</t>
+          <t>Cinema International Release 1 Seat</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>16</v>
+        <v>1600</v>
       </c>
       <c r="D42" t="n">
-        <v>14</v>
+        <v>1400</v>
       </c>
       <c r="E42" t="n">
-        <v>18</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="43">
@@ -1329,17 +1329,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Preschool (or Kindergarten), Full Day, Private, Monthly for 1 Child</t>
+          <t>Preschool or Kindergarten Full Day Private Monthly for 1 Child</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>456</v>
+        <v>45600</v>
       </c>
       <c r="D43" t="n">
-        <v>230</v>
+        <v>23000</v>
       </c>
       <c r="E43" t="n">
-        <v>1037</v>
+        <v>103700</v>
       </c>
     </row>
     <row r="44">
@@ -1350,17 +1350,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>International Primary School, Yearly for 1 Child</t>
+          <t>International Primary School Yearly for 1 Child</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>18250</v>
+        <v>1825000</v>
       </c>
       <c r="D44" t="n">
-        <v>16000</v>
+        <v>1600000</v>
       </c>
       <c r="E44" t="n">
-        <v>24000</v>
+        <v>2400000</v>
       </c>
     </row>
     <row r="45">
@@ -1371,17 +1371,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>1 Pair of Jeans (Levis 501 Or Similar)</t>
+          <t>1 Pair of Jeans Levis 501 Or Similar</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>97.23999999999999</v>
+        <v>9724</v>
       </c>
       <c r="D45" t="n">
-        <v>55</v>
+        <v>5500</v>
       </c>
       <c r="E45" t="n">
-        <v>110</v>
+        <v>11000</v>
       </c>
     </row>
     <row r="46">
@@ -1392,17 +1392,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>1 Summer Dress in a Chain Store (Zara, H&amp;M, ...)</t>
+          <t xml:space="preserve">1 Summer Dress in a Chain Store Zara HM </t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>48.76</v>
+        <v>4876</v>
       </c>
       <c r="D46" t="n">
-        <v>40</v>
+        <v>4000</v>
       </c>
       <c r="E46" t="n">
-        <v>65</v>
+        <v>6500</v>
       </c>
     </row>
     <row r="47">
@@ -1413,17 +1413,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>1 Pair of Nike Running Shoes (Mid-Range)</t>
+          <t>1 Pair of Nike Running Shoes MidRange</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>102.35</v>
+        <v>10235</v>
       </c>
       <c r="D47" t="n">
-        <v>79</v>
+        <v>7900</v>
       </c>
       <c r="E47" t="n">
-        <v>130</v>
+        <v>13000</v>
       </c>
     </row>
     <row r="48">
@@ -1438,13 +1438,13 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>148.71</v>
+        <v>14871</v>
       </c>
       <c r="D48" t="n">
-        <v>110</v>
+        <v>11000</v>
       </c>
       <c r="E48" t="n">
-        <v>160</v>
+        <v>16000</v>
       </c>
     </row>
     <row r="49">
@@ -1455,17 +1455,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Apartment (1 bedroom) in City Centre</t>
+          <t>Apartment 1 bedroom in City Centre</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1067.24</v>
+        <v>106724</v>
       </c>
       <c r="D49" t="n">
-        <v>899</v>
+        <v>89900</v>
       </c>
       <c r="E49" t="n">
-        <v>1250</v>
+        <v>125000</v>
       </c>
     </row>
     <row r="50">
@@ -1476,17 +1476,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Apartment (1 bedroom) Outside of Centre</t>
+          <t>Apartment 1 bedroom Outside of Centre</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>851.29</v>
+        <v>85129</v>
       </c>
       <c r="D50" t="n">
-        <v>650</v>
+        <v>65000</v>
       </c>
       <c r="E50" t="n">
-        <v>1000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="51">
@@ -1497,17 +1497,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Apartment (3 bedrooms) in City Centre</t>
+          <t>Apartment 3 bedrooms in City Centre</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1722.26</v>
+        <v>172226</v>
       </c>
       <c r="D51" t="n">
-        <v>1500</v>
+        <v>150000</v>
       </c>
       <c r="E51" t="n">
-        <v>2000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="52">
@@ -1518,17 +1518,17 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Apartment (3 bedrooms) Outside of Centre</t>
+          <t>Apartment 3 bedrooms Outside of Centre</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>1414.06</v>
+        <v>141406</v>
       </c>
       <c r="D52" t="n">
-        <v>1100</v>
+        <v>110000</v>
       </c>
       <c r="E52" t="n">
-        <v>1650</v>
+        <v>165000</v>
       </c>
     </row>
     <row r="53">
@@ -1543,13 +1543,13 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>7657.88</v>
+        <v>765788</v>
       </c>
       <c r="D53" t="n">
-        <v>6000</v>
+        <v>600000</v>
       </c>
       <c r="E53" t="n">
-        <v>9000</v>
+        <v>900000</v>
       </c>
     </row>
     <row r="54">
@@ -1564,13 +1564,13 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>5163.25</v>
+        <v>516325</v>
       </c>
       <c r="D54" t="n">
-        <v>3500</v>
+        <v>350000</v>
       </c>
       <c r="E54" t="n">
-        <v>6000</v>
+        <v>600000</v>
       </c>
     </row>
     <row r="55">
@@ -1581,17 +1581,17 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Average Monthly Net Salary (After Tax)</t>
+          <t>Average Monthly Net Salary After Tax</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>2874.72</v>
+        <v>287472</v>
       </c>
       <c r="D55" t="n">
-        <v>2874.72</v>
+        <v>287472</v>
       </c>
       <c r="E55" t="n">
-        <v>2874.72</v>
+        <v>287472</v>
       </c>
     </row>
     <row r="56">
@@ -1602,17 +1602,17 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Mortgage Interest Rate in Percentages (%), Yearly, for 20 Years Fixed-Rate</t>
+          <t>Mortgage Interest Rate in Percentages  Yearly for 20 Years FixedRate</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>3.66</v>
+        <v>366</v>
       </c>
       <c r="D56" t="n">
-        <v>1.25</v>
+        <v>125</v>
       </c>
       <c r="E56" t="n">
-        <v>4.5</v>
+        <v>450</v>
       </c>
     </row>
   </sheetData>

</xml_diff>